<commit_message>
More changes for serology
</commit_message>
<xml_diff>
--- a/src/database/Observation Identifiers.xlsx
+++ b/src/database/Observation Identifiers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\immregistries\IIS-Sandbox\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCB5321-E619-45B5-9C2D-6597A6F77864}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A02B3-9F22-411B-8385-2E9809476E87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1986C6D7-C5CA-4599-BFCE-3F86FDEAD719}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1986C6D7-C5CA-4599-BFCE-3F86FDEAD719}"/>
   </bookViews>
   <sheets>
     <sheet name="LOINC" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="315">
   <si>
     <t>29768-9</t>
   </si>
@@ -971,6 +971,12 @@
   </si>
   <si>
     <t>Sars-CoV-2 (finding)</t>
+  </si>
+  <si>
+    <t>292508471000119105</t>
+  </si>
+  <si>
+    <t>History of SARS-CoV-2</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1079,6 +1085,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CF1C2F-9FE9-4163-B82D-A50F4BAE4D59}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,15 +3553,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E44FC0B-EA32-456C-A20E-B67A234DC029}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
@@ -5172,6 +5179,29 @@
         <v>EQUIVOCAL("42425007", "Equivocal"),</v>
       </c>
     </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
+        <v>314</v>
+      </c>
+      <c r="D71" s="8" t="str">
+        <f t="shared" ref="D71" si="6">UPPER(C71)</f>
+        <v>HISTORY OF SARS-COV-2</v>
+      </c>
+      <c r="E71" s="7" t="str">
+        <f t="shared" ref="E71" si="7">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(D71,"&lt;"," LESS THAN "),"&gt;"," GREATER THAN "),",","_"),")","_"),"(","_"),".","_"),"#"," POUND "),"+"," PLUS ")," ","_"),"-","_")</f>
+        <v>HISTORY_OF_SARS_COV_2</v>
+      </c>
+      <c r="F71" s="8" t="str">
+        <f t="shared" ref="F71" si="8">E71&amp;"("&amp;CHAR(34)&amp;A71&amp;CHAR(34)&amp;", "&amp;CHAR(34)&amp;C71&amp;CHAR(34)&amp;"),"</f>
+        <v>HISTORY_OF_SARS_COV_2("292508471000119105", "History of SARS-CoV-2"),</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>